<commit_message>
Committing local changes before pulling updates
</commit_message>
<xml_diff>
--- a/TrueAug_SymDiGCN_WikipediaNetworksquirrel12-30-14:14:20_dir.xlsx
+++ b/TrueAug_SymDiGCN_WikipediaNetworksquirrel12-30-14:14:20_dir.xlsx
@@ -4589,7 +4589,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A64"/>
+  <dimension ref="A1:A79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4607,439 +4607,544 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Epoch: 62, Val_loss:  2.21, time:104.54, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
+          <t>Epoch: 77, Val_loss:  2.33, time:104.85, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Epoch: 61, Val_loss:  2.19, time:104.83, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
+          <t>Epoch: 76, Val_loss:  2.33, time:105.00, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Epoch: 60, Val_loss:  2.19, time:104.66, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
+          <t>Epoch: 75, Val_loss:  2.31, time:105.35, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Epoch: 59, Val_loss:  2.16, time:104.39, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
+          <t>Epoch: 74, Val_loss:  2.31, time:104.89, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Epoch: 58, Val_loss:  2.16, time:105.17, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
+          <t>Epoch: 73, Val_loss:  2.29, time:105.24, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Epoch: 57, Val_loss:  2.14, time:104.46, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
+          <t>Epoch: 72, Val_loss:  2.30, time:104.71, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Epoch: 56, Val_loss:  2.15, time:105.29, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
+          <t>Epoch: 71, Val_loss:  2.28, time:104.76, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Epoch: 55, Val_loss:  2.13, time:105.07, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
+          <t>Epoch: 70, Val_loss:  2.28, time:104.94, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Epoch: 54, Val_loss:  2.13, time:104.84, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
+          <t>Epoch: 69, Val_loss:  2.26, time:104.56, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Epoch: 53, Val_loss:  2.12, time:104.82, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
+          <t>Epoch: 68, Val_loss:  2.26, time:104.56, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Epoch: 52, Val_loss:  2.11, time:104.82, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 67, Val_loss:  2.24, time:105.64, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Epoch: 51, Val_loss:  2.10, time:104.44, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 66, Val_loss:  2.24, time:104.68, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Epoch: 50, Val_loss:  2.10, time:105.48, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 65, Val_loss:  2.22, time:104.34, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Epoch: 49, Val_loss:  2.09, time:104.56, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 64, Val_loss:  2.22, time:106.29, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Epoch: 48, Val_loss:  2.09, time:104.59, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 63, Val_loss:  2.20, time:105.29, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Epoch: 47, Val_loss:  2.08, time:104.69, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 62, Val_loss:  2.21, time:104.54, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Epoch: 46, Val_loss:  2.08, time:104.77, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 61, Val_loss:  2.19, time:104.83, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Epoch: 45, Val_loss:  2.07, time:104.61, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 60, Val_loss:  2.19, time:104.66, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Epoch: 44, Val_loss:  2.08, time:104.45, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 59, Val_loss:  2.16, time:104.39, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Epoch: 43, Val_loss:  2.06, time:104.56, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 58, Val_loss:  2.16, time:105.17, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Epoch: 42, Val_loss:  2.07, time:104.77, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 57, Val_loss:  2.14, time:104.46, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Epoch: 41, Val_loss:  2.04, time:104.84, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 56, Val_loss:  2.15, time:105.29, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Epoch: 40, Val_loss:  2.06, time:104.88, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 55, Val_loss:  2.13, time:105.07, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Epoch: 39, Val_loss:  2.03, time:105.45, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 54, Val_loss:  2.13, time:104.84, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Epoch: 38, Val_loss:  2.05, time:104.77, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 53, Val_loss:  2.12, time:104.82, test_Acc:  26.99, test_bacc:  27.81, test_f1:  18.68</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Epoch: 37, Val_loss:  2.02, time:104.74, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 52, Val_loss:  2.11, time:104.82, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Epoch: 36, Val_loss:  2.03, time:104.71, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 51, Val_loss:  2.10, time:104.44, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Epoch: 35, Val_loss:  2.00, time:104.41, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 50, Val_loss:  2.10, time:105.48, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Epoch: 34, Val_loss:  2.02, time:104.49, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 49, Val_loss:  2.09, time:104.56, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Epoch: 33, Val_loss:  1.99, time:104.21, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 48, Val_loss:  2.09, time:104.59, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Epoch: 32, Val_loss:  2.01, time:104.44, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 47, Val_loss:  2.08, time:104.69, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Epoch: 31, Val_loss:  1.98, time:104.91, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 46, Val_loss:  2.08, time:104.77, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Epoch: 30, Val_loss:  2.01, time:104.69, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 45, Val_loss:  2.07, time:104.61, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Epoch: 29, Val_loss:  1.97, time:104.78, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 44, Val_loss:  2.08, time:104.45, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Epoch: 28, Val_loss:  1.99, time:104.88, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 43, Val_loss:  2.06, time:104.56, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Epoch: 27, Val_loss:  1.96, time:104.65, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 42, Val_loss:  2.07, time:104.77, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Epoch: 26, Val_loss:  1.99, time:104.80, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 41, Val_loss:  2.04, time:104.84, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Epoch: 25, Val_loss:  1.96, time:104.66, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 40, Val_loss:  2.06, time:104.88, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Epoch: 24, Val_loss:  1.98, time:105.19, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 39, Val_loss:  2.03, time:105.45, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Epoch: 23, Val_loss:  1.96, time:104.94, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 38, Val_loss:  2.05, time:104.77, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Epoch: 22, Val_loss:  1.97, time:104.83, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 37, Val_loss:  2.02, time:104.74, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Epoch: 21, Val_loss:  1.95, time:104.57, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 36, Val_loss:  2.03, time:104.71, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Epoch: 20, Val_loss:  1.97, time:104.66, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 35, Val_loss:  2.00, time:104.41, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Epoch: 19, Val_loss:  1.95, time:104.52, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
+          <t>Epoch: 34, Val_loss:  2.02, time:104.49, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Epoch: 18, Val_loss:  1.96, time:104.41, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
+          <t>Epoch: 33, Val_loss:  1.99, time:104.21, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Epoch: 17, Val_loss:  1.95, time:104.61, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
+          <t>Epoch: 32, Val_loss:  2.01, time:104.44, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Epoch: 16, Val_loss:  1.95, time:104.74, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
+          <t>Epoch: 31, Val_loss:  1.98, time:104.91, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Epoch: 15, Val_loss:  1.96, time:104.76, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
+          <t>Epoch: 30, Val_loss:  2.01, time:104.69, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Epoch: 14, Val_loss:  1.98, time:104.68, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
+          <t>Epoch: 29, Val_loss:  1.97, time:104.78, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Epoch: 13, Val_loss:  2.00, time:104.48, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
+          <t>Epoch: 28, Val_loss:  1.99, time:104.88, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Epoch: 12, Val_loss:  2.03, time:104.89, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+          <t>Epoch: 27, Val_loss:  1.96, time:104.65, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Epoch: 11, Val_loss:  2.09, time:104.56, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+          <t>Epoch: 26, Val_loss:  1.99, time:104.80, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Epoch: 10, Val_loss:  2.15, time:104.84, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+          <t>Epoch: 25, Val_loss:  1.96, time:104.66, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Epoch:  9, Val_loss:  2.22, time:104.86, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+          <t>Epoch: 24, Val_loss:  1.98, time:105.19, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Epoch:  8, Val_loss:  2.31, time:105.09, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+          <t>Epoch: 23, Val_loss:  1.96, time:104.94, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Epoch:  7, Val_loss:  2.41, time:104.39, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+          <t>Epoch: 22, Val_loss:  1.97, time:104.83, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Epoch:  6, Val_loss:  2.52, time:104.79, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+          <t>Epoch: 21, Val_loss:  1.95, time:104.57, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Epoch:  5, Val_loss:  2.66, time:123.94, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+          <t>Epoch: 20, Val_loss:  1.97, time:104.66, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Epoch:  4, Val_loss:  2.83, time:125.11, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+          <t>Epoch: 19, Val_loss:  1.95, time:104.52, test_Acc:  24.98, test_bacc:  25.57, test_f1:  17.19</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Epoch:  3, Val_loss:  3.03, time:124.86, test_Acc:  27.38, test_bacc:  27.54, test_f1:  17.00</t>
+          <t>Epoch: 18, Val_loss:  1.96, time:104.41, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Epoch:  2, Val_loss:  3.25, time:123.21, test_Acc:  26.51, test_bacc:  26.68, test_f1:  16.29</t>
+          <t>Epoch: 17, Val_loss:  1.95, time:104.61, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Epoch:  1, Val_loss:  3.52, time:123.17, test_Acc:  24.78, test_bacc:  24.96, test_f1:  14.74</t>
+          <t>Epoch: 16, Val_loss:  1.95, time:104.74, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
+        <is>
+          <t>Epoch: 15, Val_loss:  1.96, time:104.76, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Epoch: 14, Val_loss:  1.98, time:104.68, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Epoch: 13, Val_loss:  2.00, time:104.48, test_Acc:  25.36, test_bacc:  25.81, test_f1:  18.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Epoch: 12, Val_loss:  2.03, time:104.89, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Epoch: 11, Val_loss:  2.09, time:104.56, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Epoch: 10, Val_loss:  2.15, time:104.84, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Epoch:  9, Val_loss:  2.22, time:104.86, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Epoch:  8, Val_loss:  2.31, time:105.09, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Epoch:  7, Val_loss:  2.41, time:104.39, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Epoch:  6, Val_loss:  2.52, time:104.79, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Epoch:  5, Val_loss:  2.66, time:123.94, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Epoch:  4, Val_loss:  2.83, time:125.11, test_Acc:  26.99, test_bacc:  27.15, test_f1:  17.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Epoch:  3, Val_loss:  3.03, time:124.86, test_Acc:  27.38, test_bacc:  27.54, test_f1:  17.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Epoch:  2, Val_loss:  3.25, time:123.21, test_Acc:  26.51, test_bacc:  26.68, test_f1:  16.29</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Epoch:  1, Val_loss:  3.52, time:123.17, test_Acc:  24.78, test_bacc:  24.96, test_f1:  14.74</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
         <is>
           <t>Epoch:  0, Val_loss:  3.82, time:126.09, test_Acc:  24.21, test_bacc:  24.39, test_f1:  13.83</t>
         </is>

</xml_diff>